<commit_message>
add DB sqlite and migration
</commit_message>
<xml_diff>
--- a/DB scheme.xlsx
+++ b/DB scheme.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>person</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>endDate</t>
-  </si>
-  <si>
-    <t>taskList</t>
-  </si>
-  <si>
-    <t>idCurrentTasks</t>
   </si>
   <si>
     <t>taskRegistrator</t>
@@ -505,16 +499,16 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -589,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -627,7 +621,7 @@
         <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -638,7 +632,6 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -654,15 +647,12 @@
         <v>28</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -676,22 +666,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -718,7 +708,6 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -730,13 +719,10 @@
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -756,13 +742,13 @@
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>7</v>
@@ -770,7 +756,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1"/>
     </row>
@@ -782,12 +768,12 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1"/>
     </row>
@@ -799,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>